<commit_message>
add tsv and json
</commit_message>
<xml_diff>
--- a/outputs/excel/atmosphere.xlsx
+++ b/outputs/excel/atmosphere.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,62 +422,62 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>stac_version</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>links</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>license</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>providers</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>extent</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>summaries</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>assets</t>
         </is>
@@ -548,7 +536,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{'spatial': {'bbox': [[0, -89, 360, 89]]}, 'temporal': {'interval': [['2024-03-01T00:00:00Z', '2025-12-06T00:00:00Z']]}}</t>
+          <t>{'spatial': {'bbox': [[0, -89, 360, 89]]}, 'temporal': {'interval': [['2024-03-01T00:00:00Z', '2026-02-03T00:00:00Z']]}}</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -575,79 +563,144 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>cams-global-reanalysis-eac4</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CAMS global reanalysis (EAC4)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>EAC4 (ECMWF Atmospheric Composition Reanalysis 4) is the fourth generation ECMWF global reanalysis of atmospheric composition. Reanalysis combines model data with observations from across the world into a globally complete and consistent dataset using a model of the atmosphere based on the laws of physics and chemistry. This principle, called data assimilation, is based on the method used by numerical weather prediction centres and air quality forecasting centres, where every so many hours (12 hours at ECMWF) a previous forecast is combined with newly available observations in an optimal way to produce a new best estimate of the state of the atmosphere, called analysis, from which an updated, improved forecast is issued. Reanalysis works in the same way to allow for the provision of a dataset spanning back more than a decade. Reanalysis does not have the constraint of issuing timely forecasts, so there is more time to collect observations, and when going further back in time, to allow for the ingestion of improved versions of the original observations, which all benefit the quality of the reanalysis product.
+The assimilation system is able to estimate biases between observations and to sift good-quality data from poor data. The atmosphere model allows for estimates at locations where data coverage is low or for atmospheric pollutants for which no direct observations are available. The provision of estimates at each grid point around the globe for each regular output time, over a long period, always using the same format, makes reanalysis a very convenient and popular dataset to work with.
+The observing system has changed drastically over time, and although the assimilation system can resolve data holes, the initially much sparser networks will lead to less accurate estimates. For this reason, EAC4 is only available from 2003 onwards.
+Although the analysis procedure considers chunks of data in a window of 12 hours in one go, EAC4 provides estimates every 3 hours, worldwide. This is made possible by the 4D-Var assimilation method, which takes account of the exact timing of the observations and model evolution within the assimilation window.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[{'rel': 'self', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/collections/cams-global-reanalysis-eac4'}, {'rel': 'parent', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}, {'rel': 'root', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}]</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>['Product type: Reanalysis', 'Temporal coverage: Past', 'Variable domain: Atmosphere (composition)', 'Parameter family: Aerosol', 'Parameter family: Reactive gas', 'Spatial coverage: Global', 'Variable domain: Atmosphere (meteorology)']</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>CC-BY-4.0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>[{'name': 'ECMWF'}]</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['2003-01-01T00:00:00Z', '2024-10-31T00:00:00Z']]}}</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>{'thumbnail': {'href': 'https://object-store.os-api.cci2.ecmwf.int:443/cci2-prod-catalogue/resources/cams-global-reanalysis-eac4/overview_e082c9db427fb72cdd252bf0cde444a48b36e772a19a72f1c749dc72c4a00929.png', 'type': 'image/jpg', 'roles': ['thumbnail'], 'thumborHref': 'https://ads.atmosphere.copernicus.eu/thumbnails/0GQH0j30P8Hs58k1IxHw46Yd-W0=/150x0/filters:format(webp)/object-store.os-api.cci2.ecmwf.int/cci2-prod-catalogue/resources/cams-global-reanalysis-eac4/overview_e082c9db427fb72cdd252bf0cde444a48b36e772a19a72f1c749dc72c4a00929.png'}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Collection</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.1.0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>cams-global-greenhouse-gas-inversion</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>CAMS global inversion-optimised greenhouse gas fluxes and concentrations</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>This data set contains net fluxes at the surface, atmospheric mixing ratios at model levels, and column-mean atmospheric mixing ratios  for carbon dioxide (CO2), methane (CH4) and nitrous oxide (N20).
 Natural and anthropogenic surface fluxes of greenhouse gases are key drivers of the evolution of Earth’s climate, so their monitoring is essential. Such information has been used in particular as part of the Assessment Reports of the Intergovernmental Panel on Climate Change (IPCC). Ground-based and satellite remote-sensing observations provide a means to quantifying the net fluxes between the land and ocean on the one hand and the atmosphere on the other hand. This is done through a process called atmospheric inversion, which uses transport models of the atmosphere to link the observed concentrations of CO2, CH4 and N2O to the net fluxes at the Earth's surface. By correctly modelling the winds, vertical diffusion, and convection in the global atmosphere, the observed concentrations of the greenhouse gases are used to infer the surface fluxes for the last few decades. For CH4 and N2O, the flux inversions account also for the chemical loss of these greenhouse gases. The net fluxes include contributions from the natural biosphere (e.g., vegetation, wetlands) as well anthropogenic contributions (e.g., fossil fuel emissions, rice fields).
 The data sets for the three species are updated once or three times per year adding the most recent year to the data record, while re-processing the original data record for consistency. This is reflected by the different version numbers. In addition, fluxes for methane are available based on surface air samples only or based on a combination of surface air samples and satellite observations (reflected by an 's' in the version number).</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>[{'rel': 'self', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/collections/cams-global-greenhouse-gas-inversion'}, {'rel': 'parent', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}, {'rel': 'root', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}]</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>['Product type: Reanalysis', 'Temporal coverage: Past', 'Variable domain: Atmosphere (composition)', 'Spatial coverage: Global', 'Variable domain: Emissions and surface fluxes', 'Parameter family: Greenhouse gas']</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>CC-BY-4.0</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>[{'name': 'ECMWF'}]</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['1979-01-01T00:00:00Z', '2024-12-31T00:00:00Z']]}}</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>{}</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>{'thumbnail': {'href': 'https://object-store.os-api.cci2.ecmwf.int:443/cci2-prod-catalogue/resources/cams-global-greenhouse-gas-inversion/overview_38d8bdbbbdcb2ad03e03cf6fed7c2fa885db8128b8da42dcccc57c90064c73be.png', 'type': 'image/jpg', 'roles': ['thumbnail'], 'thumborHref': 'https://ads.atmosphere.copernicus.eu/thumbnails/WPLroD78i17ktq8R1dHf4cZjqS4=/150x0/filters:format(webp)/object-store.os-api.cci2.ecmwf.int/cci2-prod-catalogue/resources/cams-global-greenhouse-gas-inversion/overview_38d8bdbbbdcb2ad03e03cf6fed7c2fa885db8128b8da42dcccc57c90064c73be.png'}}</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Collection</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>1.1.0</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>cams-europe-air-quality-reanalyses</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>CAMS European air quality reanalyses</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>This dataset provides annual air quality reanalyses for Europe based on both unvalidated and validated observations.
 CAMS produces annual air quality reanalyses for the European domain at significantly higher spatial resolution (0.1 degrees, approx. 10km) than is available from the global reanalyses. The production is currently based on an ensemble of eleven air quality data assimilation systems across Europe. A median ensemble is calculated from individual outputs, since ensemble products yield on average better performance than the individual model products. The spread between the eleven models can be used to provide an estimate of the analysis uncertainty. 
@@ -655,104 +708,39 @@
 An interim reanalysis is provided each year for the year before based on the unvalidated near-real-time observation data stream that has not undergone full quality control by the data providers yet. Once the fully quality-controlled observations are available from the data provider, typically with an additional delay of about 1 year, a final validated annual reanalysis is provided. Both reanalyses are available at hourly time steps at height levels.</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>[{'rel': 'self', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/collections/cams-europe-air-quality-reanalyses'}, {'rel': 'parent', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}, {'rel': 'root', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}]</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>['Product type: Reanalysis', 'Temporal coverage: Past', 'Variable domain: Atmosphere (composition)', 'Spatial coverage: Europe', 'Parameter family: Aerosol', 'Parameter family: Reactive gas']</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>CC-BY-4.0</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>[{'name': 'ECMWF'}]</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>{'spatial': {'bbox': [[-25, 30, 45, 72]]}, 'temporal': {'interval': [['2013-01-01T00:00:00Z', '2024-12-31T00:00:00Z']]}}</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>{}</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>{'thumbnail': {'href': 'https://object-store.os-api.cci2.ecmwf.int:443/cci2-prod-catalogue/resources/cams-europe-air-quality-reanalyses/overview_bbfe0b2e1170acdb9c1e489b34a4c7db89080f96fcde03acfdca90f450c8582a.png', 'type': 'image/jpg', 'roles': ['thumbnail'], 'thumborHref': 'https://ads.atmosphere.copernicus.eu/thumbnails/hORcB-2-fPkJl9Rl56kwVLzdVtk=/150x0/filters:format(webp)/object-store.os-api.cci2.ecmwf.int/cci2-prod-catalogue/resources/cams-europe-air-quality-reanalyses/overview_bbfe0b2e1170acdb9c1e489b34a4c7db89080f96fcde03acfdca90f450c8582a.png'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Collection</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.1.0</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>cams-global-reanalysis-eac4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CAMS global reanalysis (EAC4)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>EAC4 (ECMWF Atmospheric Composition Reanalysis 4) is the fourth generation ECMWF global reanalysis of atmospheric composition. Reanalysis combines model data with observations from across the world into a globally complete and consistent dataset using a model of the atmosphere based on the laws of physics and chemistry. This principle, called data assimilation, is based on the method used by numerical weather prediction centres and air quality forecasting centres, where every so many hours (12 hours at ECMWF) a previous forecast is combined with newly available observations in an optimal way to produce a new best estimate of the state of the atmosphere, called analysis, from which an updated, improved forecast is issued. Reanalysis works in the same way to allow for the provision of a dataset spanning back more than a decade. Reanalysis does not have the constraint of issuing timely forecasts, so there is more time to collect observations, and when going further back in time, to allow for the ingestion of improved versions of the original observations, which all benefit the quality of the reanalysis product.
-The assimilation system is able to estimate biases between observations and to sift good-quality data from poor data. The atmosphere model allows for estimates at locations where data coverage is low or for atmospheric pollutants for which no direct observations are available. The provision of estimates at each grid point around the globe for each regular output time, over a long period, always using the same format, makes reanalysis a very convenient and popular dataset to work with.
-The observing system has changed drastically over time, and although the assimilation system can resolve data holes, the initially much sparser networks will lead to less accurate estimates. For this reason, EAC4 is only available from 2003 onwards.
-Although the analysis procedure considers chunks of data in a window of 12 hours in one go, EAC4 provides estimates every 3 hours, worldwide. This is made possible by the 4D-Var assimilation method, which takes account of the exact timing of the observations and model evolution within the assimilation window.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>[{'rel': 'self', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/collections/cams-global-reanalysis-eac4'}, {'rel': 'parent', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}, {'rel': 'root', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}]</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>['Product type: Reanalysis', 'Temporal coverage: Past', 'Variable domain: Atmosphere (composition)', 'Parameter family: Aerosol', 'Parameter family: Reactive gas', 'Spatial coverage: Global', 'Variable domain: Atmosphere (meteorology)']</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>CC-BY-4.0</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>[{'name': 'ECMWF'}]</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['2003-01-01T00:00:00Z', '2024-10-31T00:00:00Z']]}}</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>{'thumbnail': {'href': 'https://object-store.os-api.cci2.ecmwf.int:443/cci2-prod-catalogue/resources/cams-global-reanalysis-eac4/overview_e082c9db427fb72cdd252bf0cde444a48b36e772a19a72f1c749dc72c4a00929.png', 'type': 'image/jpg', 'roles': ['thumbnail'], 'thumborHref': 'https://ads.atmosphere.copernicus.eu/thumbnails/0GQH0j30P8Hs58k1IxHw46Yd-W0=/150x0/filters:format(webp)/object-store.os-api.cci2.ecmwf.int/cci2-prod-catalogue/resources/cams-global-reanalysis-eac4/overview_e082c9db427fb72cdd252bf0cde444a48b36e772a19a72f1c749dc72c4a00929.png'}}</t>
         </is>
       </c>
     </row>
@@ -822,7 +810,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{'spatial': {'bbox': [[-25, 30, 45, 72]]}, 'temporal': {'interval': [['2024-01-17T00:00:00Z', '2025-12-06T00:00:00Z']]}}</t>
+          <t>{'spatial': {'bbox': [[-25, 30, 45, 72]]}, 'temporal': {'interval': [['2024-01-17T00:00:00Z', '2026-02-03T00:00:00Z']]}}</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -966,7 +954,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['2003-01-01T00:00:00Z', '2025-12-05T00:00:00Z']]}}</t>
+          <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['2003-01-01T00:00:00Z', '2025-12-03T00:00:00Z']]}}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1165,7 +1153,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['2015-01-01T00:00:00Z', '2025-12-06T00:00:00Z']]}}</t>
+          <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['2015-01-01T00:00:00Z', '2026-02-03T00:00:00Z']]}}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1391,30 +1379,29 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>cams-global-reanalysis-eac4-monthly</t>
+          <t>cams-solar-radiation-timeseries</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>CAMS global reanalysis (EAC4) monthly averaged fields</t>
+          <t>CAMS solar radiation time-series</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>EAC4 (ECMWF Atmospheric Composition Reanalysis 4) is the fourth generation ECMWF global reanalysis of atmospheric composition. Reanalysis combines model data with observations from across the world into a globally complete and consistent dataset using a model of the atmosphere based on the laws of physics and chemistry. This principle, called data assimilation, is based on the method used by numerical weather prediction centres and air quality forecasting centres, where every so many hours (12 hours at ECMWF) a previous forecast is combined with newly available observations in an optimal way to produce a new best estimate of the state of the atmosphere, called analysis, from which an updated, improved forecast is issued. Reanalysis works in the same way to allow for the provision of a dataset spanning back more than a decade. Reanalysis does not have the constraint of issuing timely forecasts, so there is more time to collect observations, and when going further back in time, to allow for the ingestion of improved versions of the original observations, which all benefit the quality of the reanalysis product.
-The assimilation system is able to estimate biases between observations and to sift good-quality data from poor data. The atmosphere model allows for estimates at locations where data coverage is low or for atmospheric pollutants for which no direct observations are available. The provision of estimates at each grid point around the globe for each regular output time, over a long period, always using the same format, makes reanalysis a very convenient and popular dataset to work with.
-The observing system has changed drastically over time, and although the assimilation system can resolve data holes, the initially much sparser networks will lead to less accurate estimates. For this reason, EAC4 is only available from 2003 onwards.
-Although the analysis procedure considers chunks of data in a window of 12 hours in one go, EAC4 provides estimates every 3 hours, worldwide. This is made possible by the 4D-Var assimilation method, which takes account of the exact timing of the observations and model evolution within the assimilation window.</t>
+          <t>The CAMS solar radiation services provide historical values (2004 to present) of global (GHI), direct (BHI) and diffuse (DHI) solar irradiation, as well as direct normal irradiation (BNI). The aim is to fulfil the needs of European and national policy development and the requirements of both commercial and public downstream services, e.g. for planning, monitoring, efficiency improvements and the integration of solar energy systems into energy supply grids.
+For clear-sky conditions, an irradiation time series is provided for any location in the world using information on aerosol, ozone and water vapour from the CAMS global forecasting system. Other properties, such as ground albedo and ground elevation, are also taken into account. Similar time series are available for cloudy (or “all sky”) conditions but, since the high-resolution cloud information is directly inferred from satellite observations, these are currently only available inside the field-of-view of the Meteosat Second Generation (MSG) and the Himawari satellites, which is roughly Europe, Africa, part of South America, the Atlantic Ocean, the Middle East, part of Asia, and Australia.
+Data is offered in both ASCII and netCDF format. Additionally, an ASCII "expert mode" format can be selected which contains in addition to the irradiation, all the input data used in their calculation (aerosol optical properties, water vapour concentration, etc). This additional information is only meaningful in the time frame at which the calculation is performed and so is only available at 1-minute time steps in universal time (UT).</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[{'rel': 'self', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/collections/cams-global-reanalysis-eac4-monthly'}, {'rel': 'parent', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}, {'rel': 'root', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}]</t>
+          <t>[{'rel': 'self', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/collections/cams-solar-radiation-timeseries'}, {'rel': 'parent', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}, {'rel': 'root', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['Product type: Reanalysis', 'Temporal coverage: Past', 'Variable domain: Atmosphere (composition)', 'Parameter family: Aerosol', 'Parameter family: Reactive gas', 'Spatial coverage: Global', 'Variable domain: Atmosphere (meteorology)']</t>
+          <t>['Temporal coverage: Past', 'Spatial coverage: Global', 'Parameter family: Radiation', 'Spatial coverage: Satellite image area', 'Product type: Analysis', 'Variable domain: Solar radiation']</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1429,7 +1416,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['2003-01-01T00:00:00Z', '2023-12-31T00:00:00Z']]}}</t>
+          <t>{'spatial': {'bbox': [[0, -89, 360, 89]]}, 'temporal': {'interval': [['2004-01-01T00:00:00Z', '2026-02-01T00:00:00Z']]}}</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1439,7 +1426,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>{'thumbnail': {'href': 'https://object-store.os-api.cci2.ecmwf.int:443/cci2-prod-catalogue/resources/cams-global-reanalysis-eac4-monthly/overview_e26d2a815d3e6499bc8d18623930c253deb87757ca8df91fa99e939137d38a46.png', 'type': 'image/jpg', 'roles': ['thumbnail'], 'thumborHref': 'https://ads.atmosphere.copernicus.eu/thumbnails/N8pJ0sN-74RKO2kbYxF1ezgGlcI=/150x0/filters:format(webp)/object-store.os-api.cci2.ecmwf.int/cci2-prod-catalogue/resources/cams-global-reanalysis-eac4-monthly/overview_e26d2a815d3e6499bc8d18623930c253deb87757ca8df91fa99e939137d38a46.png'}}</t>
+          <t>{'thumbnail': {'href': 'https://object-store.os-api.cci2.ecmwf.int:443/cci2-prod-catalogue/resources/cams-solar-radiation-timeseries/overview_51b05dc9c04479bfe717483ad887ef69461fc77410257222a19775cf68790cce.png', 'type': 'image/jpg', 'roles': ['thumbnail'], 'thumborHref': 'https://ads.atmosphere.copernicus.eu/thumbnails/fmEhVM3duj-r5aYGrd_mRQto8FU=/150x0/filters:format(webp)/object-store.os-api.cci2.ecmwf.int/cci2-prod-catalogue/resources/cams-solar-radiation-timeseries/overview_51b05dc9c04479bfe717483ad887ef69461fc77410257222a19775cf68790cce.png'}}</t>
         </is>
       </c>
     </row>
@@ -1508,7 +1495,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{'spatial': {'bbox': [[-25, 30, 45, 72]]}, 'temporal': {'interval': [['2022-12-01T00:00:00Z', '2025-12-06T00:00:00Z']]}}</t>
+          <t>{'spatial': {'bbox': [[-25, 30, 45, 72]]}, 'temporal': {'interval': [['2023-01-29T00:00:00Z', '2026-02-03T00:00:00Z']]}}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1535,29 +1522,30 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>cams-solar-radiation-timeseries</t>
+          <t>cams-global-reanalysis-eac4-monthly</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CAMS solar radiation time-series</t>
+          <t>CAMS global reanalysis (EAC4) monthly averaged fields</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>The CAMS solar radiation services provide historical values (2004 to present) of global (GHI), direct (BHI) and diffuse (DHI) solar irradiation, as well as direct normal irradiation (BNI). The aim is to fulfil the needs of European and national policy development and the requirements of both commercial and public downstream services, e.g. for planning, monitoring, efficiency improvements and the integration of solar energy systems into energy supply grids.
-For clear-sky conditions, an irradiation time series is provided for any location in the world using information on aerosol, ozone and water vapour from the CAMS global forecasting system. Other properties, such as ground albedo and ground elevation, are also taken into account. Similar time series are available for cloudy (or “all sky”) conditions but, since the high-resolution cloud information is directly inferred from satellite observations, these are currently only available inside the field-of-view of the Meteosat Second Generation (MSG) and the Himawari satellites, which is roughly Europe, Africa, part of South America, the Atlantic Ocean, the Middle East, part of Asia, and Australia.
-Data is offered in both ASCII and netCDF format. Additionally, an ASCII "expert mode" format can be selected which contains in addition to the irradiation, all the input data used in their calculation (aerosol optical properties, water vapour concentration, etc). This additional information is only meaningful in the time frame at which the calculation is performed and so is only available at 1-minute time steps in universal time (UT).</t>
+          <t>EAC4 (ECMWF Atmospheric Composition Reanalysis 4) is the fourth generation ECMWF global reanalysis of atmospheric composition. Reanalysis combines model data with observations from across the world into a globally complete and consistent dataset using a model of the atmosphere based on the laws of physics and chemistry. This principle, called data assimilation, is based on the method used by numerical weather prediction centres and air quality forecasting centres, where every so many hours (12 hours at ECMWF) a previous forecast is combined with newly available observations in an optimal way to produce a new best estimate of the state of the atmosphere, called analysis, from which an updated, improved forecast is issued. Reanalysis works in the same way to allow for the provision of a dataset spanning back more than a decade. Reanalysis does not have the constraint of issuing timely forecasts, so there is more time to collect observations, and when going further back in time, to allow for the ingestion of improved versions of the original observations, which all benefit the quality of the reanalysis product.
+The assimilation system is able to estimate biases between observations and to sift good-quality data from poor data. The atmosphere model allows for estimates at locations where data coverage is low or for atmospheric pollutants for which no direct observations are available. The provision of estimates at each grid point around the globe for each regular output time, over a long period, always using the same format, makes reanalysis a very convenient and popular dataset to work with.
+The observing system has changed drastically over time, and although the assimilation system can resolve data holes, the initially much sparser networks will lead to less accurate estimates. For this reason, EAC4 is only available from 2003 onwards.
+Although the analysis procedure considers chunks of data in a window of 12 hours in one go, EAC4 provides estimates every 3 hours, worldwide. This is made possible by the 4D-Var assimilation method, which takes account of the exact timing of the observations and model evolution within the assimilation window.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[{'rel': 'self', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/collections/cams-solar-radiation-timeseries'}, {'rel': 'parent', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}, {'rel': 'root', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}]</t>
+          <t>[{'rel': 'self', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/collections/cams-global-reanalysis-eac4-monthly'}, {'rel': 'parent', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}, {'rel': 'root', 'type': 'application/json', 'href': 'https://ads.atmosphere.copernicus.eu/api/catalogue/v1/'}]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['Temporal coverage: Past', 'Spatial coverage: Global', 'Parameter family: Radiation', 'Spatial coverage: Satellite image area', 'Product type: Analysis', 'Variable domain: Solar radiation']</t>
+          <t>['Product type: Reanalysis', 'Temporal coverage: Past', 'Variable domain: Atmosphere (composition)', 'Parameter family: Aerosol', 'Parameter family: Reactive gas', 'Spatial coverage: Global', 'Variable domain: Atmosphere (meteorology)']</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1572,7 +1560,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{'spatial': {'bbox': [[0, -89, 360, 89]]}, 'temporal': {'interval': [['2004-01-01T00:00:00Z', '2025-12-05T00:00:00Z']]}}</t>
+          <t>{'spatial': {'bbox': [[-180, -90, 180, 90]]}, 'temporal': {'interval': [['2003-01-01T00:00:00Z', '2023-12-31T00:00:00Z']]}}</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1582,7 +1570,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>{'thumbnail': {'href': 'https://object-store.os-api.cci2.ecmwf.int:443/cci2-prod-catalogue/resources/cams-solar-radiation-timeseries/overview_51b05dc9c04479bfe717483ad887ef69461fc77410257222a19775cf68790cce.png', 'type': 'image/jpg', 'roles': ['thumbnail'], 'thumborHref': 'https://ads.atmosphere.copernicus.eu/thumbnails/fmEhVM3duj-r5aYGrd_mRQto8FU=/150x0/filters:format(webp)/object-store.os-api.cci2.ecmwf.int/cci2-prod-catalogue/resources/cams-solar-radiation-timeseries/overview_51b05dc9c04479bfe717483ad887ef69461fc77410257222a19775cf68790cce.png'}}</t>
+          <t>{'thumbnail': {'href': 'https://object-store.os-api.cci2.ecmwf.int:443/cci2-prod-catalogue/resources/cams-global-reanalysis-eac4-monthly/overview_e26d2a815d3e6499bc8d18623930c253deb87757ca8df91fa99e939137d38a46.png', 'type': 'image/jpg', 'roles': ['thumbnail'], 'thumborHref': 'https://ads.atmosphere.copernicus.eu/thumbnails/N8pJ0sN-74RKO2kbYxF1ezgGlcI=/150x0/filters:format(webp)/object-store.os-api.cci2.ecmwf.int/cci2-prod-catalogue/resources/cams-global-reanalysis-eac4-monthly/overview_e26d2a815d3e6499bc8d18623930c253deb87757ca8df91fa99e939137d38a46.png'}}</t>
         </is>
       </c>
     </row>

</xml_diff>